<commit_message>
Charts with Sqr. Mileage
</commit_message>
<xml_diff>
--- a/SqrMileage.xlsx
+++ b/SqrMileage.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27907"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\obarr\OneDrive\Documents\MA321 Consulting2020\Github\MA321-Daneshgar\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/veronicamarquez/Desktop/Dr.D Ecology Bias SC/MA321-Daneshgar/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C81BC6DA-403F-43B6-BF44-5CDAC253817E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="340" yWindow="340" windowWidth="14810" windowHeight="11400" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13980" yWindow="460" windowWidth="14820" windowHeight="11400" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="108">
   <si>
     <t>Continent</t>
   </si>
@@ -231,9 +230,6 @@
     <t>East-North Central</t>
   </si>
   <si>
-    <t>North West</t>
-  </si>
-  <si>
     <t>Mountain</t>
   </si>
   <si>
@@ -258,12 +254,6 @@
     <t>N/A</t>
   </si>
   <si>
-    <t>Multiple</t>
-  </si>
-  <si>
-    <t>META-ANALYSIS</t>
-  </si>
-  <si>
     <t>sq.mi(million mi^2)</t>
   </si>
   <si>
@@ -352,12 +342,21 @@
   </si>
   <si>
     <t>WY</t>
+  </si>
+  <si>
+    <t>NW</t>
+  </si>
+  <si>
+    <t>Regions2</t>
+  </si>
+  <si>
+    <t>Sq. mi2 (mi^2)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -413,30 +412,30 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D6750B1A-B9D4-4CAD-8A80-8B2CE77CAA7B}" name="Table1" displayName="Table1" ref="A2:B9" totalsRowShown="0">
-  <autoFilter ref="A2:B9" xr:uid="{85EB0938-C572-4861-8AD7-D97B223AC135}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:B9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A2:B9" totalsRowShown="0">
+  <autoFilter ref="A2:B9"/>
+  <sortState ref="A3:B9">
     <sortCondition ref="A2:A9"/>
   </sortState>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{9777B49F-6723-4F01-807C-BE9595CA8610}" name="Continent"/>
-    <tableColumn id="2" xr3:uid="{3D045E5A-6B57-4853-B87F-F282401A4708}" name="sq.mi(million mi^2)"/>
+    <tableColumn id="1" name="Continent"/>
+    <tableColumn id="2" name="sq.mi(million mi^2)"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{163085E2-B495-4A9C-953C-DA74F0060851}" name="Table2" displayName="Table2" ref="C1:F51" totalsRowShown="0">
-  <autoFilter ref="C1:F51" xr:uid="{FC2C2E64-9E19-49CF-98D5-FBBA1C973AF8}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="C2:D51">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="C1:F51" totalsRowShown="0">
+  <autoFilter ref="C1:F51"/>
+  <sortState ref="C2:D51">
     <sortCondition ref="C1:C51"/>
   </sortState>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{2415E2D2-FA7A-4122-AEFE-A35C39F2BEC1}" name="U.S. States"/>
-    <tableColumn id="2" xr3:uid="{67367757-6A95-4C5D-94D0-363E30CCA8BD}" name="Total Sq. mi (mi^2)"/>
-    <tableColumn id="5" xr3:uid="{3A63EE42-A6E5-4A35-BB7F-91C65A7462BC}" name="states"/>
-    <tableColumn id="6" xr3:uid="{4A5F8E2E-0690-4024-89D9-65739174D4A3}" name="totalSQM"/>
+    <tableColumn id="1" name="U.S. States"/>
+    <tableColumn id="2" name="Total Sq. mi (mi^2)"/>
+    <tableColumn id="5" name="states"/>
+    <tableColumn id="6" name="totalSQM"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -704,29 +703,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J51"/>
+  <dimension ref="A1:L51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.75" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.9140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="18.08203125" customWidth="1"/>
-    <col min="7" max="7" width="15.9140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.08203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="18" customWidth="1"/>
+    <col min="7" max="7" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.4140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -740,10 +739,10 @@
         <v>61</v>
       </c>
       <c r="E1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="F1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="G1" t="s">
         <v>60</v>
@@ -755,15 +754,21 @@
         <v>63</v>
       </c>
       <c r="J1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+        <v>73</v>
+      </c>
+      <c r="K1" t="s">
+        <v>106</v>
+      </c>
+      <c r="L1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C2" t="s">
         <v>10</v>
@@ -772,7 +777,7 @@
         <v>52423</v>
       </c>
       <c r="E2" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F2">
         <v>656424</v>
@@ -789,8 +794,14 @@
       <c r="J2">
         <v>191308</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K2" t="s">
+        <v>66</v>
+      </c>
+      <c r="L2">
+        <v>299170</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -804,7 +815,7 @@
         <v>656424</v>
       </c>
       <c r="E3" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="F3">
         <v>52423</v>
@@ -821,8 +832,14 @@
       <c r="J3">
         <v>292589</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K3" t="s">
+        <v>64</v>
+      </c>
+      <c r="L3">
+        <v>191308</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -836,7 +853,7 @@
         <v>114006</v>
       </c>
       <c r="E4" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="F4">
         <v>114006</v>
@@ -853,8 +870,14 @@
       <c r="J4">
         <v>299170</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K4" t="s">
+        <v>67</v>
+      </c>
+      <c r="L4">
+        <v>855767</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -868,7 +891,7 @@
         <v>53182</v>
       </c>
       <c r="E5" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="F5">
         <v>163707</v>
@@ -880,13 +903,19 @@
         <v>1107</v>
       </c>
       <c r="I5" t="s">
-        <v>67</v>
+        <v>105</v>
       </c>
       <c r="J5">
         <v>5469</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K5" t="s">
+        <v>71</v>
+      </c>
+      <c r="L5">
+        <v>71992</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -900,7 +929,7 @@
         <v>163707</v>
       </c>
       <c r="E6" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="F6">
         <v>104100</v>
@@ -912,13 +941,19 @@
         <v>7734</v>
       </c>
       <c r="I6" t="s">
-        <v>68</v>
-      </c>
-      <c r="J6" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+        <v>67</v>
+      </c>
+      <c r="J6">
+        <v>855767</v>
+      </c>
+      <c r="K6" t="s">
+        <v>105</v>
+      </c>
+      <c r="L6">
+        <v>5469</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -932,7 +967,7 @@
         <v>104100</v>
       </c>
       <c r="E7" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="F7">
         <v>59988</v>
@@ -944,13 +979,19 @@
         <v>371</v>
       </c>
       <c r="I7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J7">
         <v>444100</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K7" t="s">
+        <v>69</v>
+      </c>
+      <c r="L7">
+        <v>895300</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -964,7 +1005,7 @@
         <v>5544</v>
       </c>
       <c r="E8" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="F8">
         <v>6459</v>
@@ -976,13 +1017,19 @@
         <v>698</v>
       </c>
       <c r="I8" t="s">
-        <v>70</v>
-      </c>
-      <c r="J8" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+        <v>69</v>
+      </c>
+      <c r="J8">
+        <v>895300</v>
+      </c>
+      <c r="K8" t="s">
+        <v>65</v>
+      </c>
+      <c r="L8">
+        <v>292589</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>3</v>
       </c>
@@ -996,7 +1043,7 @@
         <v>2489</v>
       </c>
       <c r="E9" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="F9">
         <v>36420</v>
@@ -1008,13 +1055,19 @@
         <v>535</v>
       </c>
       <c r="I9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J9">
         <v>507900</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K9" t="s">
+        <v>70</v>
+      </c>
+      <c r="L9">
+        <v>507900</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
       <c r="C10" t="s">
         <v>18</v>
       </c>
@@ -1022,7 +1075,7 @@
         <v>59988</v>
       </c>
       <c r="E10" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="F10">
         <v>82282</v>
@@ -1034,13 +1087,19 @@
         <v>5991</v>
       </c>
       <c r="I10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J10">
         <v>71992</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K10" t="s">
+        <v>68</v>
+      </c>
+      <c r="L10">
+        <v>444100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
       <c r="C11" t="s">
         <v>19</v>
       </c>
@@ -1048,7 +1107,7 @@
         <v>59441</v>
       </c>
       <c r="E11" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="F11">
         <v>35387</v>
@@ -1060,13 +1119,13 @@
         <v>1522</v>
       </c>
       <c r="I11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J11" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
       <c r="C12" t="s">
         <v>20</v>
       </c>
@@ -1074,7 +1133,7 @@
         <v>6459</v>
       </c>
       <c r="E12" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="F12">
         <v>12407</v>
@@ -1085,14 +1144,8 @@
       <c r="H12">
         <v>36</v>
       </c>
-      <c r="I12" t="s">
-        <v>76</v>
-      </c>
-      <c r="J12" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
       <c r="C13" t="s">
         <v>21</v>
       </c>
@@ -1100,7 +1153,7 @@
         <v>83574</v>
       </c>
       <c r="E13" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="F13">
         <v>96810</v>
@@ -1111,14 +1164,8 @@
       <c r="H13">
         <v>823</v>
       </c>
-      <c r="I13" t="s">
-        <v>77</v>
-      </c>
-      <c r="J13" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
       <c r="C14" t="s">
         <v>22</v>
       </c>
@@ -1126,7 +1173,7 @@
         <v>57918</v>
       </c>
       <c r="E14" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="F14">
         <v>69709</v>
@@ -1138,7 +1185,7 @@
         <v>2325</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
       <c r="C15" t="s">
         <v>23</v>
       </c>
@@ -1146,7 +1193,7 @@
         <v>36420</v>
       </c>
       <c r="E15" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="F15">
         <v>147046</v>
@@ -1158,7 +1205,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
       <c r="C16" t="s">
         <v>24</v>
       </c>
@@ -1166,7 +1213,7 @@
         <v>56276</v>
       </c>
       <c r="E16" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="F16">
         <v>52672</v>
@@ -1186,7 +1233,7 @@
         <v>82282</v>
       </c>
       <c r="E17" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="F17">
         <v>9351</v>
@@ -1206,7 +1253,7 @@
         <v>40411</v>
       </c>
       <c r="E18" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="F18">
         <v>8722</v>
@@ -1226,7 +1273,7 @@
         <v>51843</v>
       </c>
       <c r="E19" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="F19">
         <v>121598</v>
@@ -1246,7 +1293,7 @@
         <v>35387</v>
       </c>
       <c r="E20" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="F20">
         <v>54475</v>
@@ -1266,7 +1313,7 @@
         <v>12407</v>
       </c>
       <c r="E21" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="F21">
         <v>44828</v>
@@ -1286,7 +1333,7 @@
         <v>10555</v>
       </c>
       <c r="E22" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="F22">
         <v>98386</v>
@@ -1306,7 +1353,7 @@
         <v>96810</v>
       </c>
       <c r="E23" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="F23">
         <v>3515</v>
@@ -1326,7 +1373,7 @@
         <v>86943</v>
       </c>
       <c r="E24" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="F24">
         <v>268601</v>
@@ -1346,7 +1393,7 @@
         <v>48434</v>
       </c>
       <c r="E25" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="F25">
         <v>84904</v>
@@ -1366,7 +1413,7 @@
         <v>69709</v>
       </c>
       <c r="E26" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="F26">
         <v>71303</v>
@@ -1386,7 +1433,7 @@
         <v>147046</v>
       </c>
       <c r="E27" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="F27">
         <v>65503</v>
@@ -1406,7 +1453,7 @@
         <v>77358</v>
       </c>
       <c r="E28" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F28">
         <v>97818</v>
@@ -1418,7 +1465,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="29" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="29" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C29" t="s">
         <v>37</v>
       </c>
@@ -1432,7 +1479,7 @@
         <v>761</v>
       </c>
     </row>
-    <row r="30" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="30" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C30" t="s">
         <v>38</v>
       </c>
@@ -1446,7 +1493,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="31" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="31" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C31" t="s">
         <v>39</v>
       </c>
@@ -1460,7 +1507,7 @@
         <v>1303</v>
       </c>
     </row>
-    <row r="32" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="32" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C32" t="s">
         <v>40</v>
       </c>
@@ -1474,7 +1521,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="33" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="33" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C33" t="s">
         <v>41</v>
       </c>
@@ -1488,7 +1535,7 @@
         <v>7251</v>
       </c>
     </row>
-    <row r="34" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="34" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C34" t="s">
         <v>42</v>
       </c>
@@ -1502,7 +1549,7 @@
         <v>3954</v>
       </c>
     </row>
-    <row r="35" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="35" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C35" t="s">
         <v>43</v>
       </c>
@@ -1516,7 +1563,7 @@
         <v>1710</v>
       </c>
     </row>
-    <row r="36" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="36" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C36" t="s">
         <v>44</v>
       </c>
@@ -1530,7 +1577,7 @@
         <v>3875</v>
       </c>
     </row>
-    <row r="37" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="37" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C37" t="s">
         <v>45</v>
       </c>
@@ -1544,7 +1591,7 @@
         <v>1224</v>
       </c>
     </row>
-    <row r="38" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="38" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C38" t="s">
         <v>46</v>
       </c>
@@ -1558,7 +1605,7 @@
         <v>2383</v>
       </c>
     </row>
-    <row r="39" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="39" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C39" t="s">
         <v>47</v>
       </c>
@@ -1572,7 +1619,7 @@
         <v>1239</v>
       </c>
     </row>
-    <row r="40" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="40" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C40" t="s">
         <v>48</v>
       </c>
@@ -1586,7 +1633,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="41" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="41" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C41" t="s">
         <v>49</v>
       </c>
@@ -1600,7 +1647,7 @@
         <v>1896</v>
       </c>
     </row>
-    <row r="42" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="42" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C42" t="s">
         <v>50</v>
       </c>
@@ -1614,7 +1661,7 @@
         <v>1224</v>
       </c>
     </row>
-    <row r="43" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="43" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C43" t="s">
         <v>51</v>
       </c>
@@ -1628,7 +1675,7 @@
         <v>926</v>
       </c>
     </row>
-    <row r="44" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="44" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C44" t="s">
         <v>52</v>
       </c>
@@ -1642,7 +1689,7 @@
         <v>6687</v>
       </c>
     </row>
-    <row r="45" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="45" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C45" t="s">
         <v>53</v>
       </c>
@@ -1656,7 +1703,7 @@
         <v>2736</v>
       </c>
     </row>
-    <row r="46" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="46" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C46" t="s">
         <v>54</v>
       </c>
@@ -1670,7 +1717,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="47" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="47" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C47" t="s">
         <v>55</v>
       </c>
@@ -1684,7 +1731,7 @@
         <v>3171</v>
       </c>
     </row>
-    <row r="48" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="48" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C48" t="s">
         <v>56</v>
       </c>
@@ -1698,7 +1745,7 @@
         <v>4721</v>
       </c>
     </row>
-    <row r="49" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="49" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C49" t="s">
         <v>57</v>
       </c>
@@ -1712,7 +1759,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="50" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="50" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C50" t="s">
         <v>58</v>
       </c>
@@ -1726,7 +1773,7 @@
         <v>11190</v>
       </c>
     </row>
-    <row r="51" spans="3:8" x14ac:dyDescent="0.35">
+    <row r="51" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C51" t="s">
         <v>59</v>
       </c>

</xml_diff>